<commit_message>
layout adjusted to Fabio's comments
- removed drill holes for battery and lora board
- increased thickness on long traces (Vout2, 5V_SW)
</commit_message>
<xml_diff>
--- a/BOM_PCB_v2_0.xlsx
+++ b/BOM_PCB_v2_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lizvs\Documents\GitHub\iot4ag-lorawan-adc-buffer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFD22517-F8CC-45D7-956B-8D863563074C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4A8A89-96D3-4380-A9CC-8E6B975075C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-4428" windowWidth="30936" windowHeight="16896" xr2:uid="{63C7D89A-C345-47B5-8694-44AB71E4DE1D}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15870" xr2:uid="{63C7D89A-C345-47B5-8694-44AB71E4DE1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,12 +35,251 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="73">
+  <si>
+    <t>Designator</t>
+  </si>
+  <si>
+    <t>Footprint</t>
+  </si>
+  <si>
+    <t>JLCPCB Part #</t>
+  </si>
+  <si>
+    <t>Digikey part #</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>C_0805_2012Metric_Pad1.18x1.45mm_HandSolder</t>
+  </si>
+  <si>
+    <t>C111662</t>
+  </si>
+  <si>
+    <t>10u</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>D_SOD-323_HandSoldering</t>
+  </si>
+  <si>
+    <t>C85200</t>
+  </si>
+  <si>
+    <t>TSOT-23-5</t>
+  </si>
+  <si>
+    <t>C61006</t>
+  </si>
+  <si>
+    <t>C146681</t>
+  </si>
+  <si>
+    <t>R_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>C176204</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C1, C15, C20</t>
+  </si>
+  <si>
+    <t>C2, C4, C8, C11, C13, C16, C18</t>
+  </si>
+  <si>
+    <t>C3, C7, C9, C12, C14, C17, C19</t>
+  </si>
+  <si>
+    <t>C5, C6</t>
+  </si>
+  <si>
+    <t>CR1, CR2, CR3</t>
+  </si>
+  <si>
+    <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D14</t>
+  </si>
+  <si>
+    <t>D11, D12, D13</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J3, J4</t>
+  </si>
+  <si>
+    <t>R1, R3, R5</t>
+  </si>
+  <si>
+    <t>R2, R4, R6</t>
+  </si>
+  <si>
+    <t>R7, R9, R11</t>
+  </si>
+  <si>
+    <t>R8, R10, R12</t>
+  </si>
+  <si>
+    <t>RG0, RG1, RG2</t>
+  </si>
+  <si>
+    <t>SW1, SW2</t>
+  </si>
+  <si>
+    <t>U1, U4, U6</t>
+  </si>
+  <si>
+    <t>U2, U5, U7</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>U8, U9, U10</t>
+  </si>
+  <si>
+    <t>10n</t>
+  </si>
+  <si>
+    <t>0.1u</t>
+  </si>
+  <si>
+    <t>1u</t>
+  </si>
+  <si>
+    <t>330u</t>
+  </si>
+  <si>
+    <t>LM234DT</t>
+  </si>
+  <si>
+    <t>ESD9B3.3ST5G</t>
+  </si>
+  <si>
+    <t>Screw_Terminal_01x12</t>
+  </si>
+  <si>
+    <t>Conn_01x13_Pin</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>68k</t>
+  </si>
+  <si>
+    <t>SW_DIP_x03</t>
+  </si>
+  <si>
+    <t>AD8226</t>
+  </si>
+  <si>
+    <t>AD8615</t>
+  </si>
+  <si>
+    <t>ADP7142AUJZ-3.3</t>
+  </si>
+  <si>
+    <t>ohms</t>
+  </si>
+  <si>
+    <t>ALD1116SAL</t>
+  </si>
+  <si>
+    <t>CP_Elec_10x10</t>
+  </si>
+  <si>
+    <t>C1848754</t>
+  </si>
+  <si>
+    <t>C520009</t>
+  </si>
+  <si>
+    <t>C76633</t>
+  </si>
+  <si>
+    <t>D_SOD-123</t>
+  </si>
+  <si>
+    <t>C180849</t>
+  </si>
+  <si>
+    <t>R_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>C865614</t>
+  </si>
+  <si>
+    <t>SMD-6P,6.2x8.6mm DIP Switches ROHS</t>
+  </si>
+  <si>
+    <t>C976354</t>
+  </si>
+  <si>
+    <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>C521307</t>
+  </si>
+  <si>
+    <t>C403864</t>
+  </si>
+  <si>
+    <t>C157402</t>
+  </si>
+  <si>
+    <t>SOIC-8</t>
+  </si>
+  <si>
+    <t>C7420318</t>
+  </si>
+  <si>
+    <t>1N4148W</t>
+  </si>
+  <si>
+    <t>1014-1047-ND</t>
+  </si>
+  <si>
+    <t>A140876CT-ND</t>
+  </si>
+  <si>
+    <t>A140883CT-ND</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -66,8 +305,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,12 +627,395 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC35EDD-E4FE-462B-892C-47B96ADE0403}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="34.140625" customWidth="1"/>
+    <col min="2" max="2" width="44.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2">
+        <v>10</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="2">
+        <v>4120</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="2">
+        <v>41200</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>